<commit_message>
Parallal running with testNG and skip
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS977\Desktop\NopCommerceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC775B57-5134-4413-BCC2-CC61FC2D8568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26814304-73B5-4E82-BDBF-705192916C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{4ED519CE-8ACB-48DF-BFB5-CC5693CAB075}"/>
   </bookViews>
@@ -60,19 +60,19 @@
     <t>Test</t>
   </si>
   <si>
-    <t>newtestusers1@mail.com</t>
-  </si>
-  <si>
-    <t>newtestusers2@mail.com</t>
-  </si>
-  <si>
-    <t>newtestusers3@mail.com</t>
-  </si>
-  <si>
-    <t>newtestusers4@mail.com</t>
-  </si>
-  <si>
-    <t>newtestusers5@mail.com</t>
+    <t>a@mail.com</t>
+  </si>
+  <si>
+    <t>b@mail.com</t>
+  </si>
+  <si>
+    <t>c@mail.com</t>
+  </si>
+  <si>
+    <t>d@mail.com</t>
+  </si>
+  <si>
+    <t>e@mail.com</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
My account customer info and addresses page automation
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS977\Desktop\NopCommerceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26814304-73B5-4E82-BDBF-705192916C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66753608-00D3-4A00-A0CD-74F3095D4EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{4ED519CE-8ACB-48DF-BFB5-CC5693CAB075}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="2" xr2:uid="{4ED519CE-8ACB-48DF-BFB5-CC5693CAB075}"/>
   </bookViews>
   <sheets>
     <sheet name="registrationinfo" sheetId="1" r:id="rId1"/>
+    <sheet name="customerinfo" sheetId="2" r:id="rId2"/>
+    <sheet name="addresses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>FirstName</t>
   </si>
@@ -73,6 +75,48 @@
   </si>
   <si>
     <t>e@mail.com</t>
+  </si>
+  <si>
+    <t>testuser001@mail.com</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>State / province</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>House 1, Road 1, District 1</t>
+  </si>
+  <si>
+    <t>Zip / postal code</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>+1(205)555-3890</t>
+  </si>
+  <si>
+    <t>User999</t>
+  </si>
+  <si>
+    <t>a1@mail.com</t>
   </si>
 </sst>
 </file>
@@ -117,9 +161,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0DF6B0-9D11-48A3-AD92-F1EA372839F3}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,4 +616,163 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEE1726-53D1-4292-B897-13C78B415485}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E7DA3ED3-537C-4967-8B2C-5A8B5A6111E7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17206A4-B4B1-40F9-961F-70DB9A3F6DA0}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.90625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2">
+        <v>35213</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2">
+        <v>35213</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{253B84A4-1D52-4077-A7E5-790DBD8C0ED5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{9D0970EF-B574-4AFD-AB37-BB69EC1E9FA0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>